<commit_message>
update cong viec lan 1
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -65,6 +65,9 @@
     <t>14/2/2024</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t xml:space="preserve">     Logo</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
     <t>Table content</t>
   </si>
   <si>
+    <t>17/2/2024</t>
+  </si>
+  <si>
     <t>hoang (hiếu)</t>
   </si>
   <si>
@@ -129,6 +135,9 @@
   </si>
   <si>
     <t>footer</t>
+  </si>
+  <si>
+    <t>drak-light</t>
   </si>
 </sst>
 </file>
@@ -137,8 +146,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="mm/dd"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -182,6 +191,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -189,14 +212,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,7 +234,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,16 +248,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,7 +295,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,9 +303,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -288,44 +335,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -371,187 +380,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -671,8 +680,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,21 +726,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -718,30 +736,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -757,163 +751,178 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -970,9 +979,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1270,7 +1276,7 @@
   <dimension ref="A1:K986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
@@ -1311,13 +1317,13 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="24"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" ht="21.75" customHeight="1" collapsed="1" spans="1:11">
       <c r="A2" s="5" t="s">
@@ -1343,12 +1349,14 @@
       <c r="I2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24"/>
+      <c r="J2" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" spans="1:11">
       <c r="A3" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1356,7 +1364,7 @@
         <v>0.5</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6">
@@ -1366,14 +1374,14 @@
         <v>0.5</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" spans="1:11">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6">
         <v>43608</v>
@@ -1386,7 +1394,7 @@
         <v>0.9</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6">
@@ -1397,14 +1405,14 @@
         <v>0.9</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="J4" s="24"/>
+      <c r="K4" s="23"/>
     </row>
     <row r="5" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" spans="1:11">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="16">
         <v>43608</v>
@@ -1416,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="6">
@@ -1426,14 +1434,14 @@
         <v>1</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="23"/>
     </row>
     <row r="6" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" spans="1:11">
       <c r="A6" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="16">
         <v>43636</v>
@@ -1445,7 +1453,7 @@
         <v>0.9</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="6">
@@ -1455,14 +1463,14 @@
         <v>0.9</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" ht="9" hidden="1" customHeight="1" outlineLevel="2" spans="1:11">
       <c r="A7" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="16">
         <v>43641</v>
@@ -1474,7 +1482,7 @@
         <v>0.8</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="6">
@@ -1484,14 +1492,14 @@
         <v>0.8</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="26"/>
-      <c r="K7" s="24"/>
+        <v>17</v>
+      </c>
+      <c r="J7" s="25"/>
+      <c r="K7" s="23"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6">
         <v>45384</v>
@@ -1511,12 +1519,14 @@
       <c r="I8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="24"/>
+      <c r="J8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="23"/>
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:11">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1526,12 +1536,12 @@
       <c r="G9" s="6"/>
       <c r="H9" s="18"/>
       <c r="I9" s="9"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" ht="14.25" customHeight="1" spans="1:11">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6">
         <v>45384</v>
@@ -1545,18 +1555,18 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="24"/>
+        <v>26</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:11">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1566,12 +1576,12 @@
       <c r="G11" s="6"/>
       <c r="H11" s="18"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:11">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" s="6">
         <v>45384</v>
@@ -1591,12 +1601,14 @@
       <c r="I12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="25"/>
-      <c r="K12" s="24"/>
+      <c r="J12" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" ht="13" customHeight="1" spans="1:11">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1606,12 +1618,12 @@
       <c r="G13" s="6"/>
       <c r="H13" s="18"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" ht="14.25" customHeight="1" spans="1:11">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6">
         <v>45384</v>
@@ -1621,22 +1633,22 @@
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="24"/>
+        <v>26</v>
+      </c>
+      <c r="J14" s="24"/>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:11">
       <c r="A15" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" s="6">
         <v>45384</v>
@@ -1645,23 +1657,23 @@
         <v>10</v>
       </c>
       <c r="D15" s="17"/>
-      <c r="E15" s="21" t="s">
-        <v>30</v>
+      <c r="E15" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" s="25"/>
-      <c r="K15" s="24"/>
+        <v>32</v>
+      </c>
+      <c r="J15" s="24"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" ht="14.25" customHeight="1" spans="1:11">
       <c r="A16" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="6">
         <v>45384</v>
@@ -1671,22 +1683,22 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="25"/>
-      <c r="K16" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="J16" s="24"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:11">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6">
         <v>45384</v>
@@ -1702,14 +1714,14 @@
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="24"/>
+      <c r="J17" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" s="6">
         <v>45384</v>
@@ -1719,20 +1731,46 @@
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J18" s="25"/>
-      <c r="K18" s="24"/>
+        <v>32</v>
+      </c>
+      <c r="J18" s="24"/>
+      <c r="K18" s="23"/>
     </row>
-    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1" spans="1:11">
+      <c r="A19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="6">
+        <v>45384</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="17"/>
+      <c r="E19" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="18"/>
+      <c r="I19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="23"/>
+    </row>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
     <row r="22" ht="14.25" customHeight="1"/>
@@ -2702,32 +2740,42 @@
     <row r="986" ht="14.25" customHeight="1"/>
   </sheetData>
   <conditionalFormatting sqref="D18">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+      <formula>0.99</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
+  <conditionalFormatting sqref="H19">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D17">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H17">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 D4:D15">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2 H4:H15">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="greaterThan">
       <formula>0.99</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update lan 2 truoc khi chuan bi nop
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -131,10 +131,13 @@
     <t>quỳnh</t>
   </si>
   <si>
+    <t>quỳnh(hiếu)</t>
+  </si>
+  <si>
     <t>Stay Updated!</t>
   </si>
   <si>
-    <t>hoàng</t>
+    <t>hoàng(hiếu)</t>
   </si>
   <si>
     <t>back to top button</t>
@@ -157,8 +160,8 @@
     <numFmt numFmtId="176" formatCode="mm/dd"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -213,9 +216,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,6 +239,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -237,45 +261,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,6 +283,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -296,10 +298,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,7 +331,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -341,14 +352,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -389,31 +392,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,151 +554,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,6 +704,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -716,20 +728,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -741,21 +750,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -783,151 +777,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1285,7 +1288,7 @@
   <dimension ref="A1:K986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6333333333333" defaultRowHeight="15" customHeight="1"/>
@@ -1578,7 +1581,9 @@
       <c r="I10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="24"/>
+      <c r="J10" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="K10" s="23"/>
     </row>
     <row r="11" ht="14.25" customHeight="1" spans="1:11">
@@ -1588,12 +1593,18 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="18"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="24"/>
+      <c r="I11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="K11" s="23"/>
     </row>
     <row r="12" ht="14.25" customHeight="1" spans="1:11">
@@ -1670,7 +1681,9 @@
       <c r="I14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="24"/>
+      <c r="J14" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="K14" s="23"/>
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:11">
@@ -1693,7 +1706,7 @@
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J15" s="24" t="s">
         <v>14</v>
@@ -1702,7 +1715,7 @@
     </row>
     <row r="16" ht="14.25" customHeight="1" spans="1:11">
       <c r="A16" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6">
         <v>45384</v>
@@ -1712,7 +1725,7 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6" t="s">
@@ -1720,14 +1733,16 @@
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="K16" s="23"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" spans="1:11">
       <c r="A17" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6">
         <v>45384</v>
@@ -1744,13 +1759,13 @@
       <c r="H17" s="18"/>
       <c r="I17" s="9"/>
       <c r="J17" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="K17" s="23"/>
     </row>
     <row r="18" ht="14.25" customHeight="1" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="6">
         <v>45384</v>
@@ -1760,7 +1775,7 @@
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6" t="s">
@@ -1768,14 +1783,16 @@
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="J18" s="24"/>
+        <v>36</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>14</v>
+      </c>
       <c r="K18" s="23"/>
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:11">
       <c r="A19" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" s="6">
         <v>45384</v>

</xml_diff>